<commit_message>
TOUT fonctionne sauf toolbar buttons
</commit_message>
<xml_diff>
--- a/bd_fournisseurs.xlsx
+++ b/bd_fournisseurs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_mou\Desktop\Compta\compta_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E5C10B-E9E8-4A91-BFFC-0F55CA40DF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618F7428-40CC-464E-90F7-27707D2421B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,36 +112,6 @@
     <t>F109</t>
   </si>
   <si>
-    <t>Fournisseur_01</t>
-  </si>
-  <si>
-    <t>Fournisseur_02</t>
-  </si>
-  <si>
-    <t>Fournisseur_03</t>
-  </si>
-  <si>
-    <t>Fournisseur_04</t>
-  </si>
-  <si>
-    <t>Fournisseur_05</t>
-  </si>
-  <si>
-    <t>Fournisseur_06</t>
-  </si>
-  <si>
-    <t>Fournisseur_07</t>
-  </si>
-  <si>
-    <t>Fournisseur_08</t>
-  </si>
-  <si>
-    <t>Fournisseur_09</t>
-  </si>
-  <si>
-    <t>Fournisseur_10</t>
-  </si>
-  <si>
     <t>Responsable_01</t>
   </si>
   <si>
@@ -539,6 +509,36 @@
   </si>
   <si>
     <t>Test fournisseur 10</t>
+  </si>
+  <si>
+    <t>Leroy</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Mercier</t>
+  </si>
+  <si>
+    <t>Moreau</t>
+  </si>
+  <si>
+    <t>Muller</t>
+  </si>
+  <si>
+    <t>Petit</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Rousseau</t>
+  </si>
+  <si>
+    <t>Stéphane</t>
   </si>
 </sst>
 </file>
@@ -608,18 +608,23 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -649,10 +654,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -667,7 +668,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4433DBA1-2D98-4229-B406-FBE09092D07E}" name="Tableau1" displayName="Tableau1" ref="A1:T11" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4433DBA1-2D98-4229-B406-FBE09092D07E}" name="Tableau1" displayName="Tableau1" ref="A1:T11" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:T11" xr:uid="{4433DBA1-2D98-4229-B406-FBE09092D07E}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{FE514C0E-3D29-4166-AA12-241DA21314CE}" name="Code fournisseur"/>
@@ -677,7 +678,7 @@
     <tableColumn id="5" xr3:uid="{F20DA6BA-52B4-4FD4-82E6-E8B9A2A923AB}" name="NPA/Ville"/>
     <tableColumn id="6" xr3:uid="{79877B28-3D17-470C-9220-028B4D91D700}" name="No téléphone 1"/>
     <tableColumn id="7" xr3:uid="{F694454E-FB60-4384-9065-E18534F5A229}" name="No téléphone 2"/>
-    <tableColumn id="8" xr3:uid="{434F426B-0601-4BDA-9E6B-8A3C1FF6056B}" name="Site internet" dataDxfId="1" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="8" xr3:uid="{434F426B-0601-4BDA-9E6B-8A3C1FF6056B}" name="Site internet" dataDxfId="0" dataCellStyle="Lien hypertexte"/>
     <tableColumn id="9" xr3:uid="{DC4C8AEF-83BE-4E78-944E-78E5D9EE3DD6}" name="E-mail"/>
     <tableColumn id="10" xr3:uid="{73EF80BC-3005-40E0-9145-607F39C6D41A}" name="Compte à créditer"/>
     <tableColumn id="11" xr3:uid="{596F2C18-D0B6-47CF-890D-ED2B7A3386CC}" name="Compte à débiter"/>
@@ -984,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T1" sqref="A1:T1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,560 +1078,560 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" t="s">
         <v>80</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>90</v>
       </c>
-      <c r="J2" t="s">
-        <v>100</v>
-      </c>
       <c r="K2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" t="s">
         <v>101</v>
       </c>
-      <c r="L2" t="s">
-        <v>111</v>
-      </c>
       <c r="M2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" t="s">
         <v>113</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>123</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>133</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>143</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>153</v>
-      </c>
-      <c r="T2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>61</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" t="s">
         <v>81</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>91</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" t="s">
         <v>101</v>
       </c>
-      <c r="K3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L3" t="s">
-        <v>111</v>
-      </c>
       <c r="M3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="O3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" t="s">
         <v>114</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>124</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>134</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>144</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>154</v>
-      </c>
-      <c r="T3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" t="s">
         <v>82</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>92</v>
       </c>
-      <c r="J4" t="s">
-        <v>102</v>
-      </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="L4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="O4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P4" t="s">
         <v>115</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>125</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>135</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>145</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>155</v>
-      </c>
-      <c r="T4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>63</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" t="s">
         <v>83</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>93</v>
       </c>
-      <c r="J5" t="s">
-        <v>103</v>
-      </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="L5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="O5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" t="s">
         <v>116</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>126</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>136</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>146</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>156</v>
-      </c>
-      <c r="T5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" t="s">
         <v>84</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>94</v>
       </c>
-      <c r="J6" t="s">
-        <v>104</v>
-      </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="L6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="O6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" t="s">
         <v>117</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>127</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>137</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>147</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>157</v>
-      </c>
-      <c r="T6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>55</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" t="s">
         <v>85</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>95</v>
       </c>
-      <c r="J7" t="s">
-        <v>105</v>
-      </c>
       <c r="K7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="O7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" t="s">
         <v>118</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>128</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>138</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>148</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>158</v>
-      </c>
-      <c r="T7" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>56</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" t="s">
         <v>86</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>96</v>
       </c>
-      <c r="J8" t="s">
-        <v>106</v>
-      </c>
       <c r="K8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="O8" t="s">
+        <v>109</v>
+      </c>
+      <c r="P8" t="s">
         <v>119</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>129</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>139</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>149</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>159</v>
-      </c>
-      <c r="T8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>57</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>67</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" t="s">
         <v>87</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>97</v>
       </c>
-      <c r="J9" t="s">
-        <v>107</v>
-      </c>
       <c r="K9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="L9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="O9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P9" t="s">
         <v>120</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>130</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>140</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>150</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>160</v>
-      </c>
-      <c r="T9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>68</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" t="s">
         <v>88</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>98</v>
       </c>
-      <c r="J10" t="s">
-        <v>108</v>
-      </c>
       <c r="K10" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="L10" t="s">
+        <v>101</v>
+      </c>
+      <c r="M10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
         <v>111</v>
       </c>
-      <c r="M10" t="s">
-        <v>110</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>121</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>131</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>141</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>151</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>161</v>
-      </c>
-      <c r="T10" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>69</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" t="s">
         <v>89</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>99</v>
       </c>
-      <c r="J11" t="s">
-        <v>109</v>
-      </c>
       <c r="K11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M11" t="s">
+        <v>102</v>
+      </c>
+      <c r="O11" t="s">
         <v>112</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>122</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>132</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>142</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>152</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>162</v>
-      </c>
-      <c r="T11" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>